<commit_message>
Added favicon to website
</commit_message>
<xml_diff>
--- a/2023-2.xlsx
+++ b/2023-2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cthul\Dropbox\Clases\Materia-Psicologia_Cognitiva\cognitiva-quarto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7560A5-EB04-4691-8CDB-157884C452DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F569B30C-890B-4091-8AD1-D5431E043360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-16335" windowWidth="29070" windowHeight="15750" activeTab="6" xr2:uid="{42E5D5DA-AAC2-4BE0-BEAA-CA5125AD1FF2}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{42E5D5DA-AAC2-4BE0-BEAA-CA5125AD1FF2}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="169">
   <si>
     <t>manuel.mejia@cetys.mx</t>
   </si>
@@ -366,12 +366,6 @@
     <t>- [ ] 3. Accede a los links del resto de esta página.</t>
   </si>
   <si>
-    <t>- [ ] 4. Verifica que tienes instalado Word y Excel en tu computadora.</t>
-  </si>
-  <si>
-    <t>- [ ] 5. Matén instalado [JASP](https://jasp-stats.org/download/).</t>
-  </si>
-  <si>
     <t xml:space="preserve">     - Avances.</t>
   </si>
   <si>
@@ -553,6 +547,9 @@
   </si>
   <si>
     <t>**Evaluación final (todas las unidades)**</t>
+  </si>
+  <si>
+    <t>- [ ] 4. Accede a la primera videolección de Edpuzzle en Blackboard. Verifica que cargue el video sin problemas.</t>
   </si>
 </sst>
 </file>
@@ -944,7 +941,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -958,7 +955,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -1011,13 +1008,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" t="s">
         <v>122</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>124</v>
-      </c>
-      <c r="C7" t="s">
-        <v>126</v>
       </c>
       <c r="D7" t="s">
         <v>83</v>
@@ -1025,13 +1022,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" t="s">
         <v>123</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>125</v>
-      </c>
-      <c r="C8" t="s">
-        <v>127</v>
       </c>
       <c r="D8" t="s">
         <v>82</v>
@@ -1064,8 +1061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{349607C8-1C63-41CE-AC13-5EEA6651EB98}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1095,13 +1092,11 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>107</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>108</v>
-      </c>
+      <c r="A6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1162,10 +1157,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>56</v>
@@ -1189,10 +1184,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>56</v>
@@ -1213,10 +1208,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>56</v>
@@ -1240,10 +1235,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>56</v>
@@ -1270,10 +1265,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1281,10 +1276,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
@@ -1292,10 +1287,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
@@ -1303,10 +1298,10 @@
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1366,10 +1361,10 @@
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>56</v>
@@ -1396,10 +1391,10 @@
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>56</v>
@@ -1426,10 +1421,10 @@
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>56</v>
@@ -1456,10 +1451,10 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>56</v>
@@ -1483,10 +1478,10 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>56</v>
@@ -1516,7 +1511,7 @@
         <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
@@ -1524,10 +1519,10 @@
         <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
@@ -1535,10 +1530,10 @@
         <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
@@ -1546,10 +1541,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E10" s="1" t="str">
         <f>CONCATENATE("🗒️ Documento a entregar: [Doc](", F10, ") | ")</f>
@@ -1620,10 +1615,10 @@
         <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>56</v>
@@ -1650,10 +1645,10 @@
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>56</v>
@@ -1680,10 +1675,10 @@
         <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>56</v>
@@ -1713,10 +1708,10 @@
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>56</v>
@@ -1740,10 +1735,10 @@
         <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E6" s="1"/>
     </row>
@@ -1752,10 +1747,10 @@
         <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -1763,10 +1758,10 @@
         <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -1774,10 +1769,10 @@
         <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -1785,10 +1780,10 @@
         <v>18</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -2185,8 +2180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D9E6F4C-B4FC-4775-9246-1B3D065D5387}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2222,12 +2217,12 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -2235,7 +2230,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B6">
         <v>7</v>
@@ -2243,7 +2238,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C7">
         <v>7</v>
@@ -2251,7 +2246,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -2259,7 +2254,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D9">
         <v>7</v>
@@ -2267,7 +2262,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D10">
         <v>7</v>
@@ -2275,7 +2270,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D11">
         <v>7</v>
@@ -2283,12 +2278,12 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -2296,7 +2291,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -2304,7 +2299,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C15">
         <v>3</v>
@@ -2312,7 +2307,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C16">
         <v>3</v>
@@ -2320,7 +2315,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D17">
         <v>3</v>
@@ -2328,7 +2323,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D18">
         <v>3</v>
@@ -2336,7 +2331,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D19">
         <v>3</v>
@@ -2344,12 +2339,12 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -2360,7 +2355,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C22">
         <v>3</v>
@@ -2368,7 +2363,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D23">
         <v>5</v>
@@ -2376,7 +2371,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D24">
         <v>15</v>

</xml_diff>